<commit_message>
Collision pairs non functional - needs demonstrator assistance fire a ball working
</commit_message>
<xml_diff>
--- a/Task Sheet.xlsx
+++ b/Task Sheet.xlsx
@@ -199,7 +199,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="3">
+  <fills count="5">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -209,6 +209,18 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FFC00000"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -266,7 +278,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -277,6 +289,8 @@
     <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="3" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -560,7 +574,7 @@
   <dimension ref="A1:B69"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B3" sqref="B3"/>
+      <selection activeCell="A16" sqref="A16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -583,19 +597,19 @@
       </c>
     </row>
     <row r="5" spans="1:2" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="4"/>
+      <c r="A5" s="8"/>
       <c r="B5" s="1" t="s">
         <v>2</v>
       </c>
     </row>
     <row r="6" spans="1:2" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="4"/>
+      <c r="A6" s="8"/>
       <c r="B6" s="1" t="s">
         <v>3</v>
       </c>
     </row>
     <row r="7" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="4"/>
+      <c r="A7" s="9"/>
       <c r="B7" s="2" t="s">
         <v>4</v>
       </c>
@@ -636,7 +650,7 @@
       </c>
     </row>
     <row r="16" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A16" s="4"/>
+      <c r="A16" s="9"/>
       <c r="B16" s="1" t="s">
         <v>11</v>
       </c>

</xml_diff>

<commit_message>
Gun cannon limited to 20, various  check marking of boxes on spreadsheet
</commit_message>
<xml_diff>
--- a/Task Sheet.xlsx
+++ b/Task Sheet.xlsx
@@ -574,7 +574,7 @@
   <dimension ref="A1:B69"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A16" sqref="A16"/>
+      <selection activeCell="A11" sqref="A11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -609,19 +609,19 @@
       </c>
     </row>
     <row r="7" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="9"/>
+      <c r="A7" s="8"/>
       <c r="B7" s="2" t="s">
         <v>4</v>
       </c>
     </row>
     <row r="8" spans="1:2" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A8" s="4"/>
+      <c r="A8" s="8"/>
       <c r="B8" s="1" t="s">
         <v>5</v>
       </c>
     </row>
     <row r="9" spans="1:2" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A9" s="4"/>
+      <c r="A9" s="8"/>
       <c r="B9" s="1" t="s">
         <v>6</v>
       </c>

</xml_diff>

<commit_message>
BallPool physics working on GPU
</commit_message>
<xml_diff>
--- a/Task Sheet.xlsx
+++ b/Task Sheet.xlsx
@@ -574,7 +574,7 @@
   <dimension ref="A1:B69"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B8" sqref="B8"/>
+      <selection activeCell="A22" sqref="A22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -667,13 +667,13 @@
       </c>
     </row>
     <row r="21" spans="1:2" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A21" s="9"/>
+      <c r="A21" s="8"/>
       <c r="B21" s="1" t="s">
         <v>14</v>
       </c>
     </row>
     <row r="22" spans="1:2" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A22" s="4"/>
+      <c r="A22" s="8"/>
       <c r="B22" s="2" t="s">
         <v>15</v>
       </c>

</xml_diff>

<commit_message>
more packets created and defined, various basic tasks from the task list completed
</commit_message>
<xml_diff>
--- a/Task Sheet.xlsx
+++ b/Task Sheet.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12300"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="25200" windowHeight="11850"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -199,7 +199,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="5">
+  <fills count="6">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -221,6 +221,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -278,7 +284,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="10">
+  <cellXfs count="12">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -291,6 +297,8 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -573,8 +581,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B69"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A22" sqref="A22"/>
+    <sheetView tabSelected="1" topLeftCell="A25" workbookViewId="0">
+      <selection activeCell="A42" sqref="A42"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -700,25 +708,25 @@
       </c>
     </row>
     <row r="30" spans="1:2" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A30" s="4"/>
+      <c r="A30" s="8"/>
       <c r="B30" s="1" t="s">
         <v>45</v>
       </c>
     </row>
     <row r="31" spans="1:2" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A31" s="4"/>
+      <c r="A31" s="8"/>
       <c r="B31" s="1" t="s">
         <v>19</v>
       </c>
     </row>
     <row r="32" spans="1:2" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A32" s="4"/>
+      <c r="A32" s="8"/>
       <c r="B32" s="1" t="s">
         <v>20</v>
       </c>
     </row>
     <row r="33" spans="1:2" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A33" s="4"/>
+      <c r="A33" s="10"/>
       <c r="B33" s="1" t="s">
         <v>21</v>
       </c>
@@ -730,7 +738,7 @@
       </c>
     </row>
     <row r="35" spans="1:2" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A35" s="5"/>
+      <c r="A35" s="11"/>
       <c r="B35" s="1" t="s">
         <v>23</v>
       </c>
@@ -748,7 +756,7 @@
       </c>
     </row>
     <row r="38" spans="1:2" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A38" s="4"/>
+      <c r="A38" s="8"/>
       <c r="B38" s="1" t="s">
         <v>25</v>
       </c>
@@ -772,7 +780,7 @@
       </c>
     </row>
     <row r="42" spans="1:2" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A42" s="5"/>
+      <c r="A42" s="11"/>
       <c r="B42" s="1" t="s">
         <v>29</v>
       </c>

</xml_diff>

<commit_message>
astar partial implementation, player avatar
</commit_message>
<xml_diff>
--- a/Task Sheet.xlsx
+++ b/Task Sheet.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="57" uniqueCount="51">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="58" uniqueCount="52">
   <si>
     <t>Coursework Part A:</t>
   </si>
@@ -177,6 +177,9 @@
   </si>
   <si>
     <t>Complete?</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> </t>
   </si>
 </sst>
 </file>
@@ -199,7 +202,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="6">
+  <fills count="5">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -221,12 +224,6 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FFFFFF00"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -284,7 +281,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="12">
+  <cellXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -297,8 +294,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -581,8 +577,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B69"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A25" workbookViewId="0">
-      <selection activeCell="A42" sqref="A42"/>
+    <sheetView tabSelected="1" topLeftCell="A33" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="B34" sqref="B34"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -726,7 +722,9 @@
       </c>
     </row>
     <row r="33" spans="1:2" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A33" s="10"/>
+      <c r="A33" s="8" t="s">
+        <v>51</v>
+      </c>
       <c r="B33" s="1" t="s">
         <v>21</v>
       </c>
@@ -738,7 +736,7 @@
       </c>
     </row>
     <row r="35" spans="1:2" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A35" s="11"/>
+      <c r="A35" s="10"/>
       <c r="B35" s="1" t="s">
         <v>23</v>
       </c>
@@ -780,7 +778,7 @@
       </c>
     </row>
     <row r="42" spans="1:2" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A42" s="11"/>
+      <c r="A42" s="10"/>
       <c r="B42" s="1" t="s">
         <v>29</v>
       </c>

</xml_diff>

<commit_message>
first interation, finished product astar pathing working
</commit_message>
<xml_diff>
--- a/Task Sheet.xlsx
+++ b/Task Sheet.xlsx
@@ -281,7 +281,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="11">
+  <cellXfs count="12">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -295,6 +295,7 @@
     <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -577,8 +578,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B69"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A33" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B34" sqref="B34"/>
+    <sheetView tabSelected="1" topLeftCell="A25" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="A11" sqref="A11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -637,7 +638,7 @@
       </c>
     </row>
     <row r="11" spans="1:2" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A11" s="4"/>
+      <c r="A11" s="8"/>
       <c r="B11" s="1" t="s">
         <v>8</v>
       </c>
@@ -838,7 +839,7 @@
       </c>
     </row>
     <row r="53" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A53" s="5"/>
+      <c r="A53" s="11"/>
       <c r="B53" s="1" t="s">
         <v>35</v>
       </c>

</xml_diff>